<commit_message>
* update sprint backlog
</commit_message>
<xml_diff>
--- a/doc/task10/scrum_planning.xlsx
+++ b/doc/task10/scrum_planning.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoeni\Documents\Fachhochschule\s4\softwareeng\workspace\ch.bfh.bti7081.s2016.white\trunk\doc\task10\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13035" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="13035" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="1" r:id="rId1"/>
@@ -12,12 +17,12 @@
     <sheet name="Sprint Backlog" sheetId="3" r:id="rId3"/>
     <sheet name="BurndownChart" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -263,19 +268,37 @@
   </si>
   <si>
     <t>Remaining Ressources</t>
+  </si>
+  <si>
+    <t>Stefan</t>
+  </si>
+  <si>
+    <t>JD</t>
+  </si>
+  <si>
+    <t>Roger</t>
+  </si>
+  <si>
+    <t>Sidi</t>
+  </si>
+  <si>
+    <t>Mathi-Haas</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Mathias</t>
+  </si>
+  <si>
+    <t>Dave</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,159 +321,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -469,194 +341,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -664,258 +350,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -923,10 +367,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -945,58 +389,19 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
-    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
-    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
-    <cellStyle name="Title" xfId="40" builtinId="15"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
-    <cellStyle name="Comma" xfId="46" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
-    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1005,7 +410,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="313739"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1286,21 +691,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="6" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.3333333333333" customWidth="1"/>
-    <col min="2" max="2" width="18.5533333333333" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="1" ht="19.2" customHeight="1" spans="1:2">
+    <row r="1" spans="1:2" s="9" customFormat="1" ht="19.149999999999999" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1308,65 +712,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.78" customWidth="1"/>
-    <col min="2" max="2" width="31.2" customWidth="1"/>
-    <col min="3" max="3" width="31.22" style="11" customWidth="1"/>
-    <col min="4" max="4" width="7.33333333333333" customWidth="1"/>
-    <col min="5" max="5" width="11.6666666666667" customWidth="1"/>
-    <col min="6" max="6" width="13.1066666666667" customWidth="1"/>
-    <col min="7" max="7" width="10.1066666666667" customWidth="1"/>
-    <col min="8" max="8" width="14.44" customWidth="1"/>
-    <col min="12" max="12" width="14.3" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="1" ht="25.5" spans="1:8">
+    <row r="1" spans="1:12" s="9" customFormat="1" ht="30">
       <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
@@ -1392,7 +794,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" s="10" customFormat="1" ht="51" spans="1:8">
+    <row r="2" spans="1:12" s="10" customFormat="1" ht="75">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -1408,13 +810,11 @@
       <c r="E2" s="10">
         <v>30</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
       <c r="H2" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" ht="51" spans="1:8">
+    <row r="3" spans="1:12" ht="75">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1436,7 +836,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" ht="51" spans="1:8">
+    <row r="4" spans="1:12" ht="60">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1458,7 +858,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" ht="38.25" spans="1:8">
+    <row r="5" spans="1:12" ht="45">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1480,7 +880,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" ht="51" spans="1:8">
+    <row r="6" spans="1:12" ht="60">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1502,7 +902,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" ht="38.25" spans="1:8">
+    <row r="7" spans="1:12" ht="60">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1524,7 +924,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" ht="25.5" spans="1:8">
+    <row r="8" spans="1:12" ht="45">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1544,7 +944,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" ht="25.5" spans="1:8">
+    <row r="9" spans="1:12" ht="30">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1564,7 +964,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="11:12">
+    <row r="14" spans="1:12">
       <c r="K14" s="5" t="s">
         <v>36</v>
       </c>
@@ -1572,25 +972,25 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="11:12">
+    <row r="15" spans="1:12">
       <c r="K15" s="5"/>
       <c r="L15" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="11:12">
+    <row r="16" spans="1:12">
       <c r="K16" s="5"/>
       <c r="L16" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="11:12">
+    <row r="17" spans="4:12">
       <c r="K17" s="5"/>
       <c r="L17" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="11:12">
+    <row r="18" spans="4:12">
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
@@ -1609,51 +1009,49 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="11:12">
+    <row r="20" spans="4:12">
       <c r="K20" s="5"/>
       <c r="L20" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="11:12">
+    <row r="21" spans="4:12">
       <c r="K21" s="5"/>
       <c r="L21" s="5" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.78" customWidth="1"/>
-    <col min="2" max="2" width="6.22" customWidth="1"/>
-    <col min="3" max="3" width="16.8" customWidth="1"/>
-    <col min="4" max="4" width="61.1" customWidth="1"/>
-    <col min="5" max="5" width="13.8866666666667" customWidth="1"/>
-    <col min="6" max="6" width="10.3333333333333" customWidth="1"/>
-    <col min="7" max="7" width="9.78" customWidth="1"/>
-    <col min="8" max="8" width="8.33333333333333" customWidth="1"/>
-    <col min="9" max="9" width="7.88666666666667" customWidth="1"/>
-    <col min="10" max="10" width="9.10666666666667" customWidth="1"/>
-    <col min="11" max="11" width="7.22" customWidth="1"/>
-    <col min="12" max="12" width="15.22" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="61.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1" ht="38.25" spans="1:12">
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="60">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -1693,7 +1091,7 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="5">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -1707,8 +1105,12 @@
       <c r="E2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5">
         <v>8</v>
@@ -1720,10 +1122,10 @@
       </c>
       <c r="N2">
         <f>SUM(I2:I57)</f>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="5">
         <v>1.2</v>
       </c>
@@ -1739,8 +1141,12 @@
       <c r="E3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5">
         <v>4</v>
@@ -1751,7 +1157,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5">
         <v>1.3</v>
       </c>
@@ -1767,8 +1173,12 @@
       <c r="E4" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5">
         <v>4</v>
@@ -1779,7 +1189,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:14">
       <c r="A5" s="5">
         <v>3.1</v>
       </c>
@@ -1795,8 +1205,12 @@
       <c r="E5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="H5" s="5"/>
       <c r="I5" s="6">
         <v>8</v>
@@ -1807,7 +1221,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:14">
       <c r="A6" s="5">
         <v>7.1</v>
       </c>
@@ -1823,8 +1237,12 @@
       <c r="E6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5">
         <v>4</v>
@@ -1835,7 +1253,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:14">
       <c r="A7" s="5">
         <v>7.2</v>
       </c>
@@ -1851,8 +1269,12 @@
       <c r="E7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5">
         <v>4</v>
@@ -1863,7 +1285,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" customFormat="1" spans="1:12">
+    <row r="8" spans="1:14">
       <c r="A8" s="5">
         <v>7.3</v>
       </c>
@@ -1879,8 +1301,12 @@
       <c r="E8" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5">
         <v>4</v>
@@ -1891,7 +1317,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" customFormat="1" spans="1:12">
+    <row r="9" spans="1:14">
       <c r="A9" s="5">
         <v>7.4</v>
       </c>
@@ -1907,8 +1333,12 @@
       <c r="E9" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5">
         <v>4</v>
@@ -1919,7 +1349,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" customFormat="1" spans="1:12">
+    <row r="10" spans="1:14">
       <c r="A10" s="5">
         <v>7.5</v>
       </c>
@@ -1935,8 +1365,12 @@
       <c r="E10" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5">
         <v>4</v>
@@ -1947,7 +1381,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" s="4" customFormat="1" spans="1:12">
+    <row r="11" spans="1:14" s="4" customFormat="1">
       <c r="A11" s="8">
         <v>7.6</v>
       </c>
@@ -1963,8 +1397,12 @@
       <c r="E11" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="F11" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>88</v>
+      </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8">
         <v>4</v>
@@ -1975,7 +1413,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:14">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1989,7 +1427,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:14">
       <c r="A13" s="5">
         <v>1.4</v>
       </c>
@@ -2013,7 +1451,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:14">
       <c r="A14" s="5">
         <v>3.3</v>
       </c>
@@ -2035,7 +1473,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:14">
       <c r="A15" s="5">
         <v>3.4</v>
       </c>
@@ -2061,7 +1499,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:14">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -2252,10 +1690,7 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="5">
-        <f>SUM(I2:I18)</f>
-        <v>48</v>
-      </c>
+      <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
@@ -2303,28 +1738,26 @@
       <c r="L32" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.1066666666667" customWidth="1"/>
-    <col min="3" max="3" width="14.6666666666667" customWidth="1"/>
-    <col min="4" max="4" width="14.3333333333333" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="26.4" customHeight="1" spans="1:4">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="26.45" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>78</v>
       </c>
@@ -2367,8 +1800,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Sprint planing for sprint 3
</commit_message>
<xml_diff>
--- a/doc/task10/scrum_planning.xlsx
+++ b/doc/task10/scrum_planning.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="117">
   <si>
     <t>Name</t>
   </si>
@@ -240,15 +240,6 @@
     <t>Model</t>
   </si>
   <si>
-    <t>Dashboard Bl</t>
-  </si>
-  <si>
-    <t>Bl</t>
-  </si>
-  <si>
-    <t>Reports Bl</t>
-  </si>
-  <si>
     <t>Reports Data</t>
   </si>
   <si>
@@ -324,9 +315,6 @@
     <t>Adapt class diagarm</t>
   </si>
   <si>
-    <t>working</t>
-  </si>
-  <si>
     <t>Diagramm-Typen implementieren</t>
   </si>
   <si>
@@ -337,18 +325,87 @@
   </si>
   <si>
     <t>Generate Data</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>FindBugs</t>
+  </si>
+  <si>
+    <t>Login implementieren</t>
+  </si>
+  <si>
+    <t>Report vergleichen View</t>
+  </si>
+  <si>
+    <t>Klassendiagram aktualisieren</t>
+  </si>
+  <si>
+    <t>Verschiedene Charttypen implementieren</t>
+  </si>
+  <si>
+    <t>Styling Dashboard</t>
+  </si>
+  <si>
+    <t>Styling Reports view</t>
+  </si>
+  <si>
+    <t>Styling Config View (Alarm &amp; Report)</t>
+  </si>
+  <si>
+    <t>Implement Report</t>
+  </si>
+  <si>
+    <t>JD</t>
+  </si>
+  <si>
+    <t>Implementation Report Vergleich</t>
+  </si>
+  <si>
+    <t>Report vergleichen Logik</t>
+  </si>
+  <si>
+    <t>shepd1/sprim5</t>
+  </si>
+  <si>
+    <t>shepd1/ellr</t>
+  </si>
+  <si>
+    <t>Loggingfunktion / Errorhandling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -428,29 +485,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -462,26 +519,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -811,7 +884,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -819,7 +892,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -827,7 +900,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -835,7 +908,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -843,7 +916,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -851,7 +924,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -863,7 +936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1141,20 +1214,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="4.6640625" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" customWidth="1"/>
+    <col min="3" max="3" width="37.21875" customWidth="1"/>
     <col min="4" max="4" width="61.109375" customWidth="1"/>
     <col min="5" max="5" width="13.88671875" customWidth="1"/>
-    <col min="6" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.33203125" customWidth="1"/>
     <col min="9" max="9" width="7.88671875" customWidth="1"/>
     <col min="10" max="10" width="9.109375" customWidth="1"/>
@@ -1202,10 +1276,10 @@
       </c>
     </row>
     <row r="2" spans="1:15" s="17" customFormat="1" ht="14.4" customHeight="1">
-      <c r="A2" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="18"/>
+      <c r="A2" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="25"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="5">
@@ -1224,10 +1298,10 @@
         <v>51</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5">
@@ -1262,10 +1336,10 @@
         <v>51</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5">
@@ -1296,10 +1370,10 @@
         <v>51</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5">
@@ -1330,10 +1404,10 @@
         <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="6">
@@ -1341,10 +1415,10 @@
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L6" s="16">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1364,10 +1438,10 @@
         <v>60</v>
       </c>
       <c r="F7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5">
@@ -1400,10 +1474,10 @@
         <v>60</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5">
@@ -1436,10 +1510,10 @@
         <v>60</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5">
@@ -1472,10 +1546,10 @@
         <v>60</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5">
@@ -1508,10 +1582,10 @@
         <v>60</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5">
@@ -1544,10 +1618,10 @@
         <v>71</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8">
@@ -1576,15 +1650,15 @@
       <c r="L13" s="5"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="19"/>
+      <c r="A15" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="26"/>
       <c r="N15" s="14" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="O15" s="14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1592,19 +1666,22 @@
         <v>2</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I16">
         <v>8</v>
       </c>
-      <c r="L16" s="14" t="s">
-        <v>100</v>
+      <c r="K16">
+        <v>12</v>
+      </c>
+      <c r="L16" s="19">
+        <v>0.8</v>
       </c>
       <c r="N16" s="14">
         <f>SUM(I16:I26)+O16</f>
@@ -1620,24 +1697,25 @@
         <v>2</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5">
         <v>4</v>
       </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="15" t="s">
-        <v>100</v>
+      <c r="K17" s="5">
+        <v>5</v>
+      </c>
+      <c r="L17" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1646,24 +1724,25 @@
         <v>2</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="15" t="s">
         <v>60</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5">
         <v>4</v>
       </c>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="20">
-        <v>0.5</v>
+      <c r="K18" s="5">
+        <v>6</v>
+      </c>
+      <c r="L18" s="21" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1674,16 +1753,16 @@
         <v>2</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -1704,16 +1783,16 @@
         <v>2</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>60</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -1721,9 +1800,11 @@
         <v>8</v>
       </c>
       <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="15" t="s">
-        <v>100</v>
+      <c r="K20" s="5">
+        <v>12</v>
+      </c>
+      <c r="L20" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1732,14 +1813,14 @@
         <v>2</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="15" t="s">
         <v>60</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -1747,9 +1828,11 @@
         <v>4</v>
       </c>
       <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="15" t="s">
-        <v>100</v>
+      <c r="K21" s="5">
+        <v>2</v>
+      </c>
+      <c r="L21" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1758,16 +1841,16 @@
         <v>2</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>51</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -1775,9 +1858,11 @@
         <v>8</v>
       </c>
       <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="15" t="s">
-        <v>100</v>
+      <c r="K22" s="5">
+        <v>1</v>
+      </c>
+      <c r="L22" s="16">
+        <v>0.1</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1786,14 +1871,14 @@
         <v>2</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="15" t="s">
         <v>60</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -1801,9 +1886,11 @@
         <v>2</v>
       </c>
       <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="15" t="s">
-        <v>100</v>
+      <c r="K23" s="5">
+        <v>4</v>
+      </c>
+      <c r="L23" s="16">
+        <v>0.8</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1812,14 +1899,14 @@
         <v>2</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="15" t="s">
         <v>51</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
@@ -1827,22 +1914,27 @@
         <v>8</v>
       </c>
       <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="15" t="s">
-        <v>19</v>
+      <c r="K24" s="5">
+        <v>0</v>
+      </c>
+      <c r="L24" s="16">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="5"/>
+      <c r="B25">
+        <v>2</v>
+      </c>
       <c r="C25" s="15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
@@ -1850,9 +1942,11 @@
         <v>4</v>
       </c>
       <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="15" t="s">
-        <v>19</v>
+      <c r="K25" s="5">
+        <v>12</v>
+      </c>
+      <c r="L25" s="21">
+        <v>0.8</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1884,8 +1978,10 @@
       <c r="L27" s="5"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="27"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -1899,126 +1995,272 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
+      <c r="B29" s="5">
+        <v>3</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>102</v>
+      </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+      <c r="F29" s="20" t="s">
+        <v>81</v>
+      </c>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
+      <c r="I29" s="5">
+        <v>2</v>
+      </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
+      <c r="L29" s="18">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
+      <c r="B30" s="5">
+        <v>3</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>103</v>
+      </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="F30" s="24" t="s">
+        <v>115</v>
+      </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
+      <c r="I30" s="5">
+        <v>8</v>
+      </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
+      <c r="L30" s="24" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
+      <c r="B31" s="5">
+        <v>3</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" s="10"/>
+      <c r="E31" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10">
+        <v>4</v>
+      </c>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10">
+        <v>12</v>
+      </c>
+      <c r="L31" s="21">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
+      <c r="B32" s="10">
+        <v>3</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>104</v>
+      </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
+      <c r="F32" s="20" t="s">
+        <v>81</v>
+      </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
+      <c r="I32" s="5">
+        <v>4</v>
+      </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
+      <c r="L32" s="24" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
+      <c r="B33" s="10">
+        <v>3</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>113</v>
+      </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
+      <c r="F33" s="24" t="s">
+        <v>111</v>
+      </c>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
+      <c r="I33" s="5">
+        <v>16</v>
+      </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
+      <c r="L33" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="B34" s="10">
+        <v>3</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="I34" s="10">
+        <v>2</v>
+      </c>
+      <c r="L34" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="B35" s="10">
+        <v>3</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="I35" s="10">
+        <v>8</v>
+      </c>
+      <c r="L35" s="24" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="5">
-        <v>1.4</v>
-      </c>
-      <c r="B36" s="5">
-        <v>2</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>72</v>
+      <c r="A36" s="5"/>
+      <c r="B36" s="10">
+        <v>3</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>107</v>
       </c>
       <c r="D36" s="5"/>
-      <c r="E36" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="23" t="s">
+        <v>95</v>
+      </c>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
+      <c r="I36" s="5">
+        <v>8</v>
+      </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="5" t="s">
+      <c r="L36" s="24" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="5">
-        <v>3.3</v>
-      </c>
-      <c r="B37" s="5">
-        <v>2</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>74</v>
+      <c r="A37" s="5"/>
+      <c r="B37" s="10">
+        <v>3</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>108</v>
       </c>
       <c r="D37" s="5"/>
-      <c r="E37" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="23" t="s">
+        <v>81</v>
+      </c>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="6"/>
+      <c r="I37" s="6">
+        <v>4</v>
+      </c>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="15" t="s">
+      <c r="L37" s="24" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="38" spans="1:12">
+      <c r="B38" s="10">
+        <v>3</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="I38" s="10">
+        <v>4</v>
+      </c>
+      <c r="L38" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="B39" s="10">
+        <v>3</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="E39" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="I39">
+        <v>4</v>
+      </c>
+      <c r="L39" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="B40" s="10">
+        <v>3</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="F40" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="I40" s="10">
+        <v>8</v>
+      </c>
+      <c r="L40" s="28" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2041,16 +2283,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="26.4" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>